<commit_message>
active sheet in prets.xls
</commit_message>
<xml_diff>
--- a/static/files/prets.xlsx
+++ b/static/files/prets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasoudard/workspace/beta.gouv.fr/appel/static/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08C757BA-61A3-B243-A9BF-21E0701EE1D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C67C4CE3-A563-F74E-956F-0C0E9800A1DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="840" windowWidth="27020" windowHeight="16440" activeTab="2" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
+    <workbookView xWindow="1440" yWindow="840" windowWidth="27020" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Prêts" sheetId="1" r:id="rId1"/>
@@ -621,8 +621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08021C90-1ACF-2A4C-A1B0-58A48A8F7007}">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -735,7 +735,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4880C39C-0BD9-B447-909B-7F37D33CA805}">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
manage error and warning while import data from xlsx
</commit_message>
<xml_diff>
--- a/static/files/prets.xlsx
+++ b/static/files/prets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasoudard/workspace/beta.gouv.fr/appel/static/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C67C4CE3-A563-F74E-956F-0C0E9800A1DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AF150EC-0157-984D-B4A0-5A8B5055B1FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1440" yWindow="840" windowWidth="27020" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
@@ -86,9 +86,6 @@
     <t>Région</t>
   </si>
   <si>
-    <t>Caisse des dépots et des consignations locative</t>
-  </si>
-  <si>
     <t>Autre</t>
   </si>
   <si>
@@ -98,7 +95,10 @@
     <t>Etat</t>
   </si>
   <si>
-    <t>Caisse des dépots et des consignations froncière</t>
+    <t>CDC froncière</t>
+  </si>
+  <si>
+    <t>CDC locative</t>
   </si>
 </sst>
 </file>
@@ -736,7 +736,7 @@
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -746,12 +746,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
@@ -766,21 +766,21 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="F3goROOdzxmMA9QYxdTLm5iy0VfOGrd+QYe08+4dVjC9gKazvkhYf1XXmCh273AFeiqQzHfKniXhGgnqMqpeyg==" saltValue="RL50t2brIscN2tf2LbWTtw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="W9QCR56ZXV4KPLPFAEUwO7Rnvu+v5qb4D6yrVdTzveHXSCIATwPZcG35b5QCc7bLpw89PM2BK3mIwOpa73Qywg==" saltValue="qGKiaguiGOe566OHcfttkQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
small enhancements following raphaëlle's feedback
</commit_message>
<xml_diff>
--- a/static/files/prets.xlsx
+++ b/static/files/prets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasoudard/workspace/beta.gouv.fr/appel/static/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AF150EC-0157-984D-B4A0-5A8B5055B1FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7511E51A-0E61-7345-8AEC-787274DD1A9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1440" yWindow="840" windowWidth="27020" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
@@ -38,12 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
-    <t>Numéro</t>
-  </si>
-  <si>
-    <t>Date d'octroi</t>
-  </si>
-  <si>
     <t>Ici quelques explications</t>
   </si>
   <si>
@@ -65,18 +59,9 @@
     <t>5. Vérifier le contenu téléversé dans lapplication et enrigistrer en cliquant sur le bouton 'Enregistrer et Suivant'</t>
   </si>
   <si>
-    <t>Durée</t>
-  </si>
-  <si>
-    <t>Montant</t>
-  </si>
-  <si>
     <t>Attention, en aucun cas vous ne devez modifier l'entête du tableau des prêts, cela casserait l'import des données</t>
   </si>
   <si>
-    <t>Prêteur</t>
-  </si>
-  <si>
     <t>Préciser l'identité du préteur si vous avez sélectionné 'Autre'</t>
   </si>
   <si>
@@ -99,12 +84,35 @@
   </si>
   <si>
     <t>CDC locative</t>
+  </si>
+  <si>
+    <t>Montant
+(en €)</t>
+  </si>
+  <si>
+    <t>Durée
+(en années)</t>
+  </si>
+  <si>
+    <t>Date d'octroi
+(format dd/mm/yyyy)</t>
+  </si>
+  <si>
+    <t>Numéro
+(caractères alphanuméric)</t>
+  </si>
+  <si>
+    <t>Prêteur
+(choisir dans la liste)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.00\ [$€-40C]"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -177,7 +185,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -186,11 +194,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="8">
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ [$€-40C]"/>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
@@ -298,14 +314,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CE610699-E1F9-0A4E-92A0-C2463FA7C402}" name="Table2" displayName="Table2" ref="A1:F22" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CE610699-E1F9-0A4E-92A0-C2463FA7C402}" name="Table2" displayName="Table2" ref="A1:F22" totalsRowShown="0" headerRowDxfId="7">
   <autoFilter ref="A1:F22" xr:uid="{CE610699-E1F9-0A4E-92A0-C2463FA7C402}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{C27C0725-DFC5-8941-AA1D-4AA3540CBB4A}" name="Numéro"/>
-    <tableColumn id="2" xr3:uid="{82FED836-92E4-D94B-95D2-D5F3693D5EB9}" name="Date d'octroi"/>
-    <tableColumn id="3" xr3:uid="{EC09CAB2-EF86-6D49-BC29-EA9B1F4DA654}" name="Durée"/>
-    <tableColumn id="4" xr3:uid="{6DE00705-339F-A245-8F5C-197410239E91}" name="Montant"/>
-    <tableColumn id="5" xr3:uid="{DBC9DD41-246B-3B4B-A5DC-0E0BB51834D7}" name="Prêteur"/>
+    <tableColumn id="1" xr3:uid="{C27C0725-DFC5-8941-AA1D-4AA3540CBB4A}" name="Numéro_x000a_(caractères alphanuméric)"/>
+    <tableColumn id="2" xr3:uid="{82FED836-92E4-D94B-95D2-D5F3693D5EB9}" name="Date d'octroi_x000a_(format dd/mm/yyyy)" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{EC09CAB2-EF86-6D49-BC29-EA9B1F4DA654}" name="Durée_x000a_(en années)"/>
+    <tableColumn id="4" xr3:uid="{6DE00705-339F-A245-8F5C-197410239E91}" name="Montant_x000a_(en €)" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{DBC9DD41-246B-3B4B-A5DC-0E0BB51834D7}" name="Prêteur_x000a_(choisir dans la liste)"/>
     <tableColumn id="6" xr3:uid="{31B884E1-4E72-8943-A774-4051BA0B67DD}" name="Préciser l'identité du préteur si vous avez sélectionné 'Autre'"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -313,10 +329,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{60458129-C213-8741-80B4-B15A740996D3}" name="preteurs" displayName="preteurs" ref="A1:A7" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2" totalsRowBorderDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{60458129-C213-8741-80B4-B15A740996D3}" name="preteurs" displayName="preteurs" ref="A1:A7" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A1:A7" xr:uid="{60458129-C213-8741-80B4-B15A740996D3}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{68B921AF-0801-1140-A800-5EFE7005DB88}" name="Prêteurs (Ne pas modifier)" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{68B921AF-0801-1140-A800-5EFE7005DB88}" name="Prêteurs (Ne pas modifier)" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -619,37 +635,124 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08021C90-1ACF-2A4C-A1B0-58A48A8F7007}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="20.83203125" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="20.83203125" customWidth="1"/>
     <col min="6" max="6" width="30.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>13</v>
-      </c>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B2" s="7"/>
+      <c r="D2" s="6">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B3" s="7"/>
+      <c r="D3" s="6"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B4" s="7"/>
+      <c r="D4" s="6"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B5" s="7"/>
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B6" s="7"/>
+      <c r="D6" s="6"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B7" s="7"/>
+      <c r="D7" s="6"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B8" s="7"/>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="7"/>
+      <c r="D9" s="6"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B10" s="7"/>
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B11" s="7"/>
+      <c r="D11" s="6"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B12" s="7"/>
+      <c r="D12" s="6"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B13" s="7"/>
+      <c r="D13" s="6"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B14" s="7"/>
+      <c r="D14" s="6"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B15" s="7"/>
+      <c r="D15" s="6"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B16" s="7"/>
+      <c r="D16" s="6"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B17" s="7"/>
+      <c r="D17" s="6"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B18" s="7"/>
+      <c r="D18" s="6"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B19" s="7"/>
+      <c r="D19" s="6"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B20" s="7"/>
+      <c r="D20" s="6"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B21" s="7"/>
+      <c r="D21" s="6"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B22" s="7"/>
+      <c r="D22" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -687,42 +790,42 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -746,37 +849,37 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
display 0 instead of None for number of logements
</commit_message>
<xml_diff>
--- a/static/files/prets.xlsx
+++ b/static/files/prets.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasoudard/workspace/beta.gouv.fr/appel/static/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{041FA66D-6545-CF43-A5E6-3953C8C9B696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56596778-DC71-0C40-9B95-1D22894AA23C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1780" yWindow="1560" windowWidth="27020" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
@@ -80,12 +80,6 @@
     <t>Etat</t>
   </si>
   <si>
-    <t>CDC froncière</t>
-  </si>
-  <si>
-    <t>CDC locative</t>
-  </si>
-  <si>
     <t>Montant
 (en €)</t>
   </si>
@@ -104,6 +98,12 @@
   <si>
     <t>Prêteur
 (choisir dans la liste déroulante)</t>
+  </si>
+  <si>
+    <t>CDC pour le foncier</t>
+  </si>
+  <si>
+    <t>CDC pour le logement</t>
   </si>
 </sst>
 </file>
@@ -746,19 +746,19 @@
   <sheetData>
     <row r="1" spans="1:6" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="22" t="s">
         <v>18</v>
-      </c>
-      <c r="C1" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>20</v>
       </c>
       <c r="F1" s="24" t="s">
         <v>8</v>
@@ -934,12 +934,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="F1:F2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1022,7 +1022,7 @@
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1052,12 +1052,12 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
@@ -1066,7 +1066,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="W9QCR56ZXV4KPLPFAEUwO7Rnvu+v5qb4D6yrVdTzveHXSCIATwPZcG35b5QCc7bLpw89PM2BK3mIwOpa73Qywg==" saltValue="qGKiaguiGOe566OHcfttkQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="+aALapghvuu3RA0eppu6l/4wiB8CNkPEhI9tr7nmuY3RJC+f3w2wEmCHfp+8KC5X/ckbUeAloMazA4PGXJifMw==" saltValue="zkKHIvrY1/eq3V2hbRhJsw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>